<commit_message>
+ log4j & new structure
</commit_message>
<xml_diff>
--- a/autotestSites/mail/utilities/MailTestData.xlsx
+++ b/autotestSites/mail/utilities/MailTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="7215" yWindow="1290" windowWidth="20985" windowHeight="2430"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="20985" windowHeight="5400"/>
   </bookViews>
   <sheets>
     <sheet name="RegistrationTests" sheetId="1" r:id="rId1"/>
@@ -12,11 +12,12 @@
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="77">
   <si>
     <t>firstName</t>
   </si>
@@ -244,6 +245,9 @@
   </si>
   <si>
     <t>werh3424dqw1s54GE</t>
+  </si>
+  <si>
+    <t>testCaseNumber</t>
   </si>
 </sst>
 </file>
@@ -602,635 +606,705 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="4">
+      <c r="E2" s="4">
         <v>40979</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>24</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>45</v>
-      </c>
-      <c r="G2" t="s">
-        <v>50</v>
       </c>
       <c r="H2" t="s">
         <v>50</v>
       </c>
-      <c r="I2">
+      <c r="I2" t="s">
+        <v>50</v>
+      </c>
+      <c r="J2">
         <v>1231092266</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="4">
+      <c r="E3" s="4">
         <v>40980</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>24</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>46</v>
-      </c>
-      <c r="G3" t="s">
-        <v>75</v>
       </c>
       <c r="H3" t="s">
         <v>75</v>
       </c>
-      <c r="I3">
+      <c r="I3" t="s">
+        <v>75</v>
+      </c>
+      <c r="J3">
         <v>6345123123</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="4">
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="4">
         <v>40981</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>24</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>47</v>
-      </c>
-      <c r="G4" t="s">
-        <v>73</v>
       </c>
       <c r="H4" t="s">
         <v>73</v>
       </c>
-      <c r="I4">
+      <c r="I4" t="s">
+        <v>73</v>
+      </c>
+      <c r="J4">
         <v>7456234324</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="4">
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="4">
         <v>40982</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>24</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>48</v>
-      </c>
-      <c r="G5" t="s">
-        <v>52</v>
       </c>
       <c r="H5" t="s">
         <v>52</v>
       </c>
-      <c r="I5">
+      <c r="I5" t="s">
+        <v>52</v>
+      </c>
+      <c r="J5">
         <v>1232534657</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
         <v>11</v>
       </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="4">
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="4">
         <v>40983</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>25</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>49</v>
-      </c>
-      <c r="G6" t="s">
-        <v>53</v>
       </c>
       <c r="H6" t="s">
         <v>53</v>
       </c>
-      <c r="I6">
+      <c r="I6" t="s">
+        <v>53</v>
+      </c>
+      <c r="J6">
         <v>4735353242</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="J7" s="2" t="s">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K7" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="5" t="s">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="4">
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="4">
         <v>40979</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>24</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>55</v>
-      </c>
-      <c r="G9" t="s">
-        <v>69</v>
       </c>
       <c r="H9" t="s">
         <v>69</v>
       </c>
-      <c r="I9">
+      <c r="I9" t="s">
+        <v>69</v>
+      </c>
+      <c r="J9">
         <v>1231092266</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
         <v>8</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>54</v>
       </c>
-      <c r="D10" s="4">
+      <c r="E10" s="4">
         <v>40980</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>24</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>56</v>
-      </c>
-      <c r="G10" t="s">
-        <v>70</v>
       </c>
       <c r="H10" t="s">
         <v>70</v>
       </c>
-      <c r="I10">
+      <c r="I10" t="s">
+        <v>70</v>
+      </c>
+      <c r="J10">
         <v>6345123123</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
         <v>10</v>
       </c>
-      <c r="C11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="4">
+      <c r="D11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="4">
         <v>40981</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>54</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>57</v>
-      </c>
-      <c r="G11" t="s">
-        <v>71</v>
       </c>
       <c r="H11" t="s">
         <v>71</v>
       </c>
-      <c r="I11">
+      <c r="I11" t="s">
+        <v>71</v>
+      </c>
+      <c r="J11">
         <v>1232534657</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
         <v>11</v>
       </c>
-      <c r="C12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="4">
+      <c r="D12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="4">
         <v>40982</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>25</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>54</v>
-      </c>
-      <c r="G12" t="s">
-        <v>72</v>
       </c>
       <c r="H12" t="s">
         <v>72</v>
       </c>
-      <c r="I12">
+      <c r="I12" t="s">
+        <v>72</v>
+      </c>
+      <c r="J12">
         <v>4735353242</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
         <v>15</v>
       </c>
-      <c r="C13" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="4">
+      <c r="D13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="4">
         <v>40983</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>24</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>58</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>28</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>8761234331</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
         <v>16</v>
       </c>
-      <c r="C14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="4">
+      <c r="D14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="4">
         <v>40984</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>24</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>59</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>17</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
         <v>54</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>1454623423</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>7</v>
+      </c>
+      <c r="C15" t="s">
         <v>18</v>
       </c>
-      <c r="C15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="4">
+      <c r="D15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" s="4">
         <v>40985</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>25</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>60</v>
-      </c>
-      <c r="G15" t="s">
-        <v>74</v>
       </c>
       <c r="H15" t="s">
         <v>74</v>
       </c>
       <c r="I15" t="s">
+        <v>74</v>
+      </c>
+      <c r="J15" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>8</v>
+      </c>
+      <c r="C16" t="s">
         <v>19</v>
       </c>
-      <c r="C16" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" s="4">
+      <c r="D16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" s="4">
         <v>40986</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>24</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>61</v>
-      </c>
-      <c r="G16" t="s">
-        <v>29</v>
       </c>
       <c r="H16" t="s">
         <v>29</v>
       </c>
-      <c r="I16" s="3" t="s">
+      <c r="I16" t="s">
+        <v>29</v>
+      </c>
+      <c r="J16" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="J16" s="2" t="s">
+      <c r="K16" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="K16" t="s">
+      <c r="L16" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>9</v>
+      </c>
+      <c r="C17" t="s">
         <v>20</v>
       </c>
-      <c r="C17" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" s="4">
+      <c r="D17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="4">
         <v>40987</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>24</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>62</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17" t="s">
         <v>21</v>
       </c>
-      <c r="H17" t="s">
+      <c r="I17" t="s">
         <v>14</v>
       </c>
-      <c r="I17" s="3">
+      <c r="J17" s="3">
         <v>5463423411</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>10</v>
+      </c>
+      <c r="C18" t="s">
         <v>26</v>
       </c>
-      <c r="C18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" s="4">
+      <c r="D18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" s="4">
         <v>40988</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>25</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>63</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>14</v>
       </c>
-      <c r="H18" t="s">
+      <c r="I18" t="s">
         <v>30</v>
       </c>
-      <c r="I18">
+      <c r="J18">
         <v>4123412343</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>11</v>
+      </c>
+      <c r="C19" t="s">
         <v>31</v>
       </c>
-      <c r="C19" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="4">
+      <c r="D19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" s="4">
         <v>40989</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>24</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>14</v>
-      </c>
-      <c r="G19" t="s">
-        <v>32</v>
       </c>
       <c r="H19" t="s">
         <v>32</v>
       </c>
-      <c r="I19" s="3">
+      <c r="I19" t="s">
+        <v>32</v>
+      </c>
+      <c r="J19" s="3">
         <v>1212312654</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>12</v>
+      </c>
+      <c r="C20" t="s">
         <v>33</v>
       </c>
-      <c r="C20" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" s="4">
+      <c r="D20" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" s="4">
         <v>40990</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>24</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>64</v>
-      </c>
-      <c r="G20" t="s">
-        <v>35</v>
       </c>
       <c r="H20" t="s">
         <v>35</v>
       </c>
-      <c r="I20" s="3">
+      <c r="I20" t="s">
+        <v>35</v>
+      </c>
+      <c r="J20" s="3">
         <v>11563674234235</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>13</v>
+      </c>
+      <c r="C21" t="s">
         <v>34</v>
       </c>
-      <c r="C21" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" s="4">
+      <c r="D21" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" s="4">
         <v>40991</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>24</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>65</v>
-      </c>
-      <c r="G21" t="s">
-        <v>36</v>
       </c>
       <c r="H21" t="s">
         <v>36</v>
       </c>
       <c r="I21" t="s">
+        <v>36</v>
+      </c>
+      <c r="J21" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>14</v>
+      </c>
+      <c r="C22" t="s">
         <v>41</v>
       </c>
-      <c r="C22" t="s">
-        <v>5</v>
-      </c>
-      <c r="D22" s="4">
+      <c r="D22" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22" s="4">
         <v>44196</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>25</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>66</v>
-      </c>
-      <c r="G22" t="s">
-        <v>42</v>
       </c>
       <c r="H22" t="s">
         <v>42</v>
       </c>
-      <c r="I22" s="3">
+      <c r="I22" t="s">
+        <v>42</v>
+      </c>
+      <c r="J22" s="3">
         <v>3735324324</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>15</v>
+      </c>
+      <c r="C23" t="s">
         <v>40</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>37</v>
       </c>
-      <c r="D23" s="4">
+      <c r="E23" s="4">
         <v>42084</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>24</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>38</v>
-      </c>
-      <c r="G23" t="s">
-        <v>39</v>
       </c>
       <c r="H23" t="s">
         <v>39</v>
       </c>
-      <c r="I23" s="3">
+      <c r="I23" t="s">
+        <v>39</v>
+      </c>
+      <c r="J23" s="3">
         <v>1999999999</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>16</v>
+      </c>
+      <c r="C24" t="s">
         <v>43</v>
       </c>
-      <c r="C24" t="s">
-        <v>5</v>
-      </c>
-      <c r="D24" s="4">
+      <c r="D24" t="s">
+        <v>5</v>
+      </c>
+      <c r="E24" s="4">
         <v>42084</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>25</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>67</v>
-      </c>
-      <c r="G24" t="s">
-        <v>44</v>
       </c>
       <c r="H24" t="s">
         <v>44</v>
       </c>
-      <c r="I24" s="3">
+      <c r="I24" t="s">
+        <v>44</v>
+      </c>
+      <c r="J24" s="3">
         <v>5124312312</v>
       </c>
     </row>

</xml_diff>